<commit_message>
Segundaa bateria de testes
</commit_message>
<xml_diff>
--- a/dados/salas_preferenciais_2023.2.xlsx
+++ b/dados/salas_preferenciais_2023.2.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">ADMINISTRAÇÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">207-A, 208-A, 209-A, 210-A</t>
+    <t xml:space="preserve">207-B, 208-B, 209-B, 210-B</t>
   </si>
   <si>
     <t xml:space="preserve">Separar as salas por “,”</t>
@@ -237,10 +237,10 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="101.86"/>

</xml_diff>

<commit_message>
Melhora bastante o arquivo de saida
</commit_message>
<xml_diff>
--- a/dados/salas_preferenciais_2023.2.xlsx
+++ b/dados/salas_preferenciais_2023.2.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">CIÊNCIA DA COMPUTAÇÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">305-B, 308-B, 309-B, 310-B</t>
+    <t xml:space="preserve">305-B , 308-B , 309-B , 310-B</t>
   </si>
   <si>
     <t xml:space="preserve">CIÊNCIAS SOCIAIS</t>
@@ -236,11 +236,11 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="101.86"/>

</xml_diff>

<commit_message>
salas preferenciais por disciplina
</commit_message>
<xml_diff>
--- a/dados/salas_preferenciais_2023.2.xlsx
+++ b/dados/salas_preferenciais_2023.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t xml:space="preserve">Curso/Matéria</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">301-A, 302-A, 303-A, 304-A</t>
   </si>
   <si>
+    <t xml:space="preserve">Preferências de disciplina sobrescrevem preferências de curso</t>
+  </si>
+  <si>
     <t xml:space="preserve">CIÊNCIA DA COMPUTAÇÃO</t>
   </si>
   <si>
@@ -110,6 +113,36 @@
   </si>
   <si>
     <t xml:space="preserve">202-B, 203-B, 204-B, 205-B, 206-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCB295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109-DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCH632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCH626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEX557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCH633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCH627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEX556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110-DE</t>
   </si>
 </sst>
 </file>
@@ -119,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,6 +180,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -204,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,6 +254,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,13 +278,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="101.86"/>
@@ -276,93 +320,152 @@
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementa agrupamento de disciplinas
</commit_message>
<xml_diff>
--- a/dados/salas_preferenciais_2023.2.xlsx
+++ b/dados/salas_preferenciais_2023.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Curso/Matéria</t>
   </si>
@@ -113,36 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">202-B, 203-B, 204-B, 205-B, 206-B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCB295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109-DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCH632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105-B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCH626</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEX557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCH633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCH627</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEX556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110-DE</t>
   </si>
 </sst>
 </file>
@@ -152,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,13 +150,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -244,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,10 +217,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,13 +237,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="101.86"/>
@@ -410,62 +369,6 @@
       </c>
       <c r="B14" s="0" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>